<commit_message>
Bug fix: Rows now display as expected in the excel spreadsheet.
</commit_message>
<xml_diff>
--- a/EmptyTemplate.xlsx
+++ b/EmptyTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aiden Gourley\Desktop\LettingsFinance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aiden Gourley\Desktop\MHLettingsStatementsToExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1CC5F1-BBC8-4D7E-97E0-A9C7F024F908}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F19311-0ED0-40C5-B317-F6CE685BFFA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -789,320 +789,320 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EB89157-652F-4B78-A2AF-F1BC4D3D61BC}" name="Table01" displayName="Table01" ref="A2:H15" headerRowCount="0" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EB89157-652F-4B78-A2AF-F1BC4D3D61BC}" name="Table01" displayName="Table01" ref="A2:H16" headerRowCount="0" headerRowDxfId="219" dataDxfId="218" totalsRowDxfId="217">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D146A5E6-7A4A-4F26-BA41-B33542C55ED6}" name="Column1" totalsRowLabel="Total" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{124DD348-FF14-49DE-8E5E-73C684540887}" name="Column2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{456F692C-A369-4C0B-8CD3-228860A77B66}" name="Column3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{4641AB7B-B63C-4C16-8860-CAF57EA3B099}" name="Column4" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D9569AF1-C585-4665-A058-11711A303B76}" name="Column5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{73F9DF9C-1476-4E2E-9895-38D29AA70CC7}" name="Column6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{EB851C9B-5D00-4A32-9D9B-CFED064B43A3}" name="Column7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{3489FD19-E3A6-4719-86D9-F98D46392781}" name="Column8" totalsRowFunction="count" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{D146A5E6-7A4A-4F26-BA41-B33542C55ED6}" name="Column1" totalsRowLabel="Total" dataDxfId="216"/>
+    <tableColumn id="2" xr3:uid="{124DD348-FF14-49DE-8E5E-73C684540887}" name="Column2" dataDxfId="215"/>
+    <tableColumn id="3" xr3:uid="{456F692C-A369-4C0B-8CD3-228860A77B66}" name="Column3" dataDxfId="214"/>
+    <tableColumn id="4" xr3:uid="{4641AB7B-B63C-4C16-8860-CAF57EA3B099}" name="Column4" dataDxfId="213"/>
+    <tableColumn id="5" xr3:uid="{D9569AF1-C585-4665-A058-11711A303B76}" name="Column5" dataDxfId="212"/>
+    <tableColumn id="6" xr3:uid="{73F9DF9C-1476-4E2E-9895-38D29AA70CC7}" name="Column6" dataDxfId="211"/>
+    <tableColumn id="7" xr3:uid="{EB851C9B-5D00-4A32-9D9B-CFED064B43A3}" name="Column7" dataDxfId="210"/>
+    <tableColumn id="8" xr3:uid="{3489FD19-E3A6-4719-86D9-F98D46392781}" name="Column8" totalsRowFunction="count" dataDxfId="209"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{325427CB-9A80-4997-96CE-BB5255AEFAC3}" name="Table10" displayName="Table10" ref="A2:H15" headerRowCount="0" headerRowDxfId="101" dataDxfId="99" totalsRowDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{325427CB-9A80-4997-96CE-BB5255AEFAC3}" name="Table10" displayName="Table10" ref="A2:H16" headerRowCount="0" headerRowDxfId="120" dataDxfId="119" totalsRowDxfId="118">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{72C5D1AD-D65F-4C5B-A97E-EB1857C07436}" name="Column1" totalsRowLabel="Total" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{B41CEEF4-10AB-4B9F-87B9-B3C78CB1F4DD}" name="Column2" dataDxfId="108"/>
-    <tableColumn id="3" xr3:uid="{98EAFB2F-65EB-4103-99D5-469875CFDF8B}" name="Column3" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{D55B2230-6DE3-4CFA-AC07-715A12D5575C}" name="Column4" dataDxfId="106"/>
-    <tableColumn id="5" xr3:uid="{76E4EDE4-0903-46ED-8767-160EC4BE0CCD}" name="Column5" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{E7E88165-E87F-4FFF-A4A2-43D2E63D7731}" name="Column6" dataDxfId="104"/>
-    <tableColumn id="7" xr3:uid="{4C0C2977-2ACB-4833-87E5-D44B52134D58}" name="Column7" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{09619A23-B177-4D75-936B-EE8EF25E6D4F}" name="Column8" totalsRowFunction="count" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{72C5D1AD-D65F-4C5B-A97E-EB1857C07436}" name="Column1" totalsRowLabel="Total" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{B41CEEF4-10AB-4B9F-87B9-B3C78CB1F4DD}" name="Column2" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{98EAFB2F-65EB-4103-99D5-469875CFDF8B}" name="Column3" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{D55B2230-6DE3-4CFA-AC07-715A12D5575C}" name="Column4" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{76E4EDE4-0903-46ED-8767-160EC4BE0CCD}" name="Column5" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{E7E88165-E87F-4FFF-A4A2-43D2E63D7731}" name="Column6" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{4C0C2977-2ACB-4833-87E5-D44B52134D58}" name="Column7" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{09619A23-B177-4D75-936B-EE8EF25E6D4F}" name="Column8" totalsRowFunction="count" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8DA748EF-AA94-4756-85DA-324E42622BD1}" name="Table11" displayName="Table11" ref="A2:H15" headerRowCount="0" headerRowDxfId="112" dataDxfId="110" totalsRowDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8DA748EF-AA94-4756-85DA-324E42622BD1}" name="Table11" displayName="Table11" ref="A2:H16" headerRowCount="0" headerRowDxfId="109" dataDxfId="108" totalsRowDxfId="107">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E9991992-3404-463D-95F6-031BF9F57041}" name="Column1" totalsRowLabel="Total" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{64484ACA-E2AE-4650-9AFA-093BFD0005BA}" name="Column2" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{A8538602-51F8-4008-A60A-C2B1D0588078}" name="Column3" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{9E1AD13C-8835-4A85-89DB-7D968CCFB217}" name="Column4" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{EA85CA82-C023-431C-9A14-93C8528763DE}" name="Column5" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{BE35B8F2-65F1-4097-8139-168EE00C48F0}" name="Column6" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{16FB5769-5BCB-4ED3-B1A5-F0FBA7EA5E4B}" name="Column7" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{C75F9E60-4FD6-42BF-8669-E2588BBEB4DA}" name="Column8" totalsRowFunction="count" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{E9991992-3404-463D-95F6-031BF9F57041}" name="Column1" totalsRowLabel="Total" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{64484ACA-E2AE-4650-9AFA-093BFD0005BA}" name="Column2" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{A8538602-51F8-4008-A60A-C2B1D0588078}" name="Column3" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{9E1AD13C-8835-4A85-89DB-7D968CCFB217}" name="Column4" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{EA85CA82-C023-431C-9A14-93C8528763DE}" name="Column5" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{BE35B8F2-65F1-4097-8139-168EE00C48F0}" name="Column6" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{16FB5769-5BCB-4ED3-B1A5-F0FBA7EA5E4B}" name="Column7" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{C75F9E60-4FD6-42BF-8669-E2588BBEB4DA}" name="Column8" totalsRowFunction="count" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{98913E47-F824-4975-AD4C-A9A70D636300}" name="Table12" displayName="Table12" ref="A2:H15" headerRowCount="0" headerRowDxfId="123" dataDxfId="121" totalsRowDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{98913E47-F824-4975-AD4C-A9A70D636300}" name="Table12" displayName="Table12" ref="A2:H16" headerRowCount="0" headerRowDxfId="98" dataDxfId="97" totalsRowDxfId="96">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D012E940-4F3C-42B9-87BC-BA824DA42CBF}" name="Column1" totalsRowLabel="Total" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{3439D913-8596-4B1B-B285-DE8B3278746D}" name="Column2" dataDxfId="130"/>
-    <tableColumn id="3" xr3:uid="{3D57B6E5-F836-4C86-A61B-597AECA26925}" name="Column3" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{8132C4B7-2FF3-4D8F-9D3C-2B7CAC549049}" name="Column4" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{A94D4663-946D-435A-8808-6809C66F980A}" name="Column5" dataDxfId="127"/>
-    <tableColumn id="6" xr3:uid="{685AC6D9-B5D0-4D5B-B891-D8B349ED26FE}" name="Column6" dataDxfId="126"/>
-    <tableColumn id="7" xr3:uid="{957CAFC3-0C22-45DF-BC39-BF53B4699123}" name="Column7" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{9F3CC9DC-1604-47AF-9C42-2D4DE46F364F}" name="Column8" totalsRowFunction="count" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{D012E940-4F3C-42B9-87BC-BA824DA42CBF}" name="Column1" totalsRowLabel="Total" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{3439D913-8596-4B1B-B285-DE8B3278746D}" name="Column2" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{3D57B6E5-F836-4C86-A61B-597AECA26925}" name="Column3" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{8132C4B7-2FF3-4D8F-9D3C-2B7CAC549049}" name="Column4" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{A94D4663-946D-435A-8808-6809C66F980A}" name="Column5" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{685AC6D9-B5D0-4D5B-B891-D8B349ED26FE}" name="Column6" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{957CAFC3-0C22-45DF-BC39-BF53B4699123}" name="Column7" dataDxfId="89"/>
+    <tableColumn id="8" xr3:uid="{9F3CC9DC-1604-47AF-9C42-2D4DE46F364F}" name="Column8" totalsRowFunction="count" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FDD5A518-9134-4114-A04F-F09A0486495E}" name="Table13" displayName="Table13" ref="A2:H15" headerRowCount="0" headerRowDxfId="134" dataDxfId="132" totalsRowDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FDD5A518-9134-4114-A04F-F09A0486495E}" name="Table13" displayName="Table13" ref="A2:H16" headerRowCount="0" headerRowDxfId="87" dataDxfId="86" totalsRowDxfId="85">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{01A8780F-C039-4376-A637-8C93C6AE2A59}" name="Column1" totalsRowLabel="Total" dataDxfId="142"/>
-    <tableColumn id="2" xr3:uid="{FEA91B3D-761F-475A-A3A3-CA63F29A0A99}" name="Column2" dataDxfId="141"/>
-    <tableColumn id="3" xr3:uid="{D4156C39-A322-478B-9943-C78BD1F39B15}" name="Column3" dataDxfId="140"/>
-    <tableColumn id="4" xr3:uid="{25EE66F5-04BA-4C27-85D6-0C7BC2DC1A6E}" name="Column4" dataDxfId="139"/>
-    <tableColumn id="5" xr3:uid="{157465CB-6938-48BA-B48A-710DC0052A6D}" name="Column5" dataDxfId="138"/>
-    <tableColumn id="6" xr3:uid="{05CC2ACF-AF2E-4246-90E9-99C9F364917C}" name="Column6" dataDxfId="137"/>
-    <tableColumn id="7" xr3:uid="{B607BE4D-61A6-4F97-B98D-6E2A79434E79}" name="Column7" dataDxfId="136"/>
-    <tableColumn id="8" xr3:uid="{50335F03-E425-42A6-B86C-05CD04CE49D3}" name="Column8" totalsRowFunction="count" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{01A8780F-C039-4376-A637-8C93C6AE2A59}" name="Column1" totalsRowLabel="Total" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{FEA91B3D-761F-475A-A3A3-CA63F29A0A99}" name="Column2" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{D4156C39-A322-478B-9943-C78BD1F39B15}" name="Column3" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{25EE66F5-04BA-4C27-85D6-0C7BC2DC1A6E}" name="Column4" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{157465CB-6938-48BA-B48A-710DC0052A6D}" name="Column5" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{05CC2ACF-AF2E-4246-90E9-99C9F364917C}" name="Column6" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{B607BE4D-61A6-4F97-B98D-6E2A79434E79}" name="Column7" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{50335F03-E425-42A6-B86C-05CD04CE49D3}" name="Column8" totalsRowFunction="count" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1FD7C3F1-68B3-4FA8-956B-83E2865DAE28}" name="Table14" displayName="Table14" ref="A2:H15" headerRowCount="0" headerRowDxfId="145" dataDxfId="143" totalsRowDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1FD7C3F1-68B3-4FA8-956B-83E2865DAE28}" name="Table14" displayName="Table14" ref="A2:H16" headerRowCount="0" headerRowDxfId="76" dataDxfId="75" totalsRowDxfId="74">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{55664E0C-813B-4DF2-9DB1-89CBBB502121}" name="Column1" totalsRowLabel="Total" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{04C57330-C3F3-4860-83BB-E08B7CD601A7}" name="Column2" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{5327D0BC-8164-4DDB-BA8F-404F4B218B37}" name="Column3" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{ECBEEF2E-85AE-4BAC-B1BE-65DB6D8B822B}" name="Column4" dataDxfId="150"/>
-    <tableColumn id="5" xr3:uid="{A0D80129-A0F6-4DC7-B83E-701DCBD10C3C}" name="Column5" dataDxfId="149"/>
-    <tableColumn id="6" xr3:uid="{C62087EC-01AB-4B76-85B6-429ED54281D7}" name="Column6" dataDxfId="148"/>
-    <tableColumn id="7" xr3:uid="{E3D05467-761F-44B1-8BDF-584CAECD45E5}" name="Column7" dataDxfId="147"/>
-    <tableColumn id="8" xr3:uid="{B9F8589E-85F8-4EF4-8BBE-BDEC34599CDB}" name="Column8" totalsRowFunction="count" dataDxfId="146"/>
+    <tableColumn id="1" xr3:uid="{55664E0C-813B-4DF2-9DB1-89CBBB502121}" name="Column1" totalsRowLabel="Total" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{04C57330-C3F3-4860-83BB-E08B7CD601A7}" name="Column2" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{5327D0BC-8164-4DDB-BA8F-404F4B218B37}" name="Column3" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{ECBEEF2E-85AE-4BAC-B1BE-65DB6D8B822B}" name="Column4" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{A0D80129-A0F6-4DC7-B83E-701DCBD10C3C}" name="Column5" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{C62087EC-01AB-4B76-85B6-429ED54281D7}" name="Column6" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{E3D05467-761F-44B1-8BDF-584CAECD45E5}" name="Column7" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{B9F8589E-85F8-4EF4-8BBE-BDEC34599CDB}" name="Column8" totalsRowFunction="count" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{446C1A5F-5A1B-4A27-AFDF-38A1E415E212}" name="Table15" displayName="Table15" ref="A2:H15" headerRowCount="0" headerRowDxfId="156" dataDxfId="154" totalsRowDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{446C1A5F-5A1B-4A27-AFDF-38A1E415E212}" name="Table15" displayName="Table15" ref="A2:H16" headerRowCount="0" headerRowDxfId="65" dataDxfId="64" totalsRowDxfId="63">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C29DE3F4-F5D2-452F-A1AE-B940EBBCD209}" name="Column1" totalsRowLabel="Total" dataDxfId="164"/>
-    <tableColumn id="2" xr3:uid="{B7338BB8-FF71-4F44-B6B4-563C37D6ADB9}" name="Column2" dataDxfId="163"/>
-    <tableColumn id="3" xr3:uid="{CA3D3B4B-78F8-4D10-BB74-FC720D37B42B}" name="Column3" dataDxfId="162"/>
-    <tableColumn id="4" xr3:uid="{2B9B9BEF-7035-43EA-8180-CA5C1A5C4AFB}" name="Column4" dataDxfId="161"/>
-    <tableColumn id="5" xr3:uid="{24C78D8C-EDE6-4F22-9DA2-B8F1F56226D2}" name="Column5" dataDxfId="160"/>
-    <tableColumn id="6" xr3:uid="{C732AD78-57F5-4409-A701-94C4546DB445}" name="Column6" dataDxfId="159"/>
-    <tableColumn id="7" xr3:uid="{903022A1-00A9-4D4B-84AF-41B83E0DCA69}" name="Column7" dataDxfId="158"/>
-    <tableColumn id="8" xr3:uid="{0DD3A0D8-AC6A-4DA0-837D-5368DF91F2CF}" name="Column8" totalsRowFunction="count" dataDxfId="157"/>
+    <tableColumn id="1" xr3:uid="{C29DE3F4-F5D2-452F-A1AE-B940EBBCD209}" name="Column1" totalsRowLabel="Total" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{B7338BB8-FF71-4F44-B6B4-563C37D6ADB9}" name="Column2" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{CA3D3B4B-78F8-4D10-BB74-FC720D37B42B}" name="Column3" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{2B9B9BEF-7035-43EA-8180-CA5C1A5C4AFB}" name="Column4" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{24C78D8C-EDE6-4F22-9DA2-B8F1F56226D2}" name="Column5" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{C732AD78-57F5-4409-A701-94C4546DB445}" name="Column6" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{903022A1-00A9-4D4B-84AF-41B83E0DCA69}" name="Column7" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{0DD3A0D8-AC6A-4DA0-837D-5368DF91F2CF}" name="Column8" totalsRowFunction="count" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E750518B-FA3A-4AB5-8D4B-73E504C444AC}" name="Table16" displayName="Table16" ref="A2:H15" headerRowCount="0" headerRowDxfId="167" dataDxfId="165" totalsRowDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E750518B-FA3A-4AB5-8D4B-73E504C444AC}" name="Table16" displayName="Table16" ref="A2:H16" headerRowCount="0" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{DD0C4038-00AA-4E41-8935-DD231D06A414}" name="Column1" totalsRowLabel="Total" dataDxfId="175"/>
-    <tableColumn id="2" xr3:uid="{A0314D29-4838-4EB3-940C-019A4E854BAA}" name="Column2" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{45B69F5A-E406-48C1-8049-E7053E0E6CDC}" name="Column3" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{86E913D9-6C19-4D27-AA27-3C0BF1F2BC6B}" name="Column4" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{CAE0EBE9-2A69-47D4-9D8C-93CE3C38B5EB}" name="Column5" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{B155EDD1-CD84-495A-AE85-BECA430911CE}" name="Column6" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{10E448A5-5883-4EDB-AB23-49A12387DA70}" name="Column7" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{E6E3D59C-7180-45D5-9468-F7B09B74A28F}" name="Column8" totalsRowFunction="count" dataDxfId="168"/>
+    <tableColumn id="1" xr3:uid="{DD0C4038-00AA-4E41-8935-DD231D06A414}" name="Column1" totalsRowLabel="Total" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{A0314D29-4838-4EB3-940C-019A4E854BAA}" name="Column2" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{45B69F5A-E406-48C1-8049-E7053E0E6CDC}" name="Column3" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{86E913D9-6C19-4D27-AA27-3C0BF1F2BC6B}" name="Column4" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{CAE0EBE9-2A69-47D4-9D8C-93CE3C38B5EB}" name="Column5" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{B155EDD1-CD84-495A-AE85-BECA430911CE}" name="Column6" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{10E448A5-5883-4EDB-AB23-49A12387DA70}" name="Column7" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{E6E3D59C-7180-45D5-9468-F7B09B74A28F}" name="Column8" totalsRowFunction="count" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D32C94A7-29D7-4DCC-80AC-510B0EB16D83}" name="Table17" displayName="Table17" ref="A2:H15" headerRowCount="0" headerRowDxfId="178" dataDxfId="176" totalsRowDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D32C94A7-29D7-4DCC-80AC-510B0EB16D83}" name="Table17" displayName="Table17" ref="A2:H16" headerRowCount="0" headerRowDxfId="43" dataDxfId="42" totalsRowDxfId="41">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A1FA69B8-A85E-43EE-87E0-5C24BA7F9B76}" name="Column1" totalsRowLabel="Total" dataDxfId="186"/>
-    <tableColumn id="2" xr3:uid="{F8678D7B-25F4-4C76-9E2C-5A3268BADF63}" name="Column2" dataDxfId="185"/>
-    <tableColumn id="3" xr3:uid="{DEEBB82A-E328-4F72-AC3C-94097A0F2798}" name="Column3" dataDxfId="184"/>
-    <tableColumn id="4" xr3:uid="{CE6E8D4B-F378-4C5E-98CB-9396C5F0B346}" name="Column4" dataDxfId="183"/>
-    <tableColumn id="5" xr3:uid="{318E125C-8EC0-46F8-8FEF-543BCC249A0E}" name="Column5" dataDxfId="182"/>
-    <tableColumn id="6" xr3:uid="{4A787244-89F3-4E65-A886-07B9F31EC000}" name="Column6" dataDxfId="181"/>
-    <tableColumn id="7" xr3:uid="{7B4B76C9-E71F-4512-8F4E-A10B405A1490}" name="Column7" dataDxfId="180"/>
-    <tableColumn id="8" xr3:uid="{DB24C010-74E0-4443-A736-B4BC52982324}" name="Column8" totalsRowFunction="count" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{A1FA69B8-A85E-43EE-87E0-5C24BA7F9B76}" name="Column1" totalsRowLabel="Total" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{F8678D7B-25F4-4C76-9E2C-5A3268BADF63}" name="Column2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{DEEBB82A-E328-4F72-AC3C-94097A0F2798}" name="Column3" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{CE6E8D4B-F378-4C5E-98CB-9396C5F0B346}" name="Column4" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{318E125C-8EC0-46F8-8FEF-543BCC249A0E}" name="Column5" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{4A787244-89F3-4E65-A886-07B9F31EC000}" name="Column6" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{7B4B76C9-E71F-4512-8F4E-A10B405A1490}" name="Column7" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{DB24C010-74E0-4443-A736-B4BC52982324}" name="Column8" totalsRowFunction="count" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{78A9418B-0383-4B28-B433-8BDAE2A0A6AA}" name="Table18" displayName="Table18" ref="A2:H15" headerRowCount="0" headerRowDxfId="189" dataDxfId="187" totalsRowDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{78A9418B-0383-4B28-B433-8BDAE2A0A6AA}" name="Table18" displayName="Table18" ref="A2:H16" headerRowCount="0" headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A17D8F77-7FEB-477A-BEC1-45996DBD227C}" name="Column1" totalsRowLabel="Total" dataDxfId="197"/>
-    <tableColumn id="2" xr3:uid="{6CA20319-6D2D-420D-9770-E51E8CBA9F04}" name="Column2" dataDxfId="196"/>
-    <tableColumn id="3" xr3:uid="{A64157C8-54A7-47A9-8584-60BDA2A94983}" name="Column3" dataDxfId="195"/>
-    <tableColumn id="4" xr3:uid="{C5841934-BE77-4082-9BF5-58673C632DFC}" name="Column4" dataDxfId="194"/>
-    <tableColumn id="5" xr3:uid="{15F74460-85B8-4FEC-95CA-05F9A4715F90}" name="Column5" dataDxfId="193"/>
-    <tableColumn id="6" xr3:uid="{BEC19B7B-39CF-4984-82AD-BCFCBD8D3178}" name="Column6" dataDxfId="192"/>
-    <tableColumn id="7" xr3:uid="{BE1A16E1-3524-4907-8D76-B4CDBC857D00}" name="Column7" dataDxfId="191"/>
-    <tableColumn id="8" xr3:uid="{8D51EA78-35E1-427C-B3AE-93F56E146AB2}" name="Column8" totalsRowFunction="count" dataDxfId="190"/>
+    <tableColumn id="1" xr3:uid="{A17D8F77-7FEB-477A-BEC1-45996DBD227C}" name="Column1" totalsRowLabel="Total" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{6CA20319-6D2D-420D-9770-E51E8CBA9F04}" name="Column2" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{A64157C8-54A7-47A9-8584-60BDA2A94983}" name="Column3" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{C5841934-BE77-4082-9BF5-58673C632DFC}" name="Column4" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{15F74460-85B8-4FEC-95CA-05F9A4715F90}" name="Column5" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{BEC19B7B-39CF-4984-82AD-BCFCBD8D3178}" name="Column6" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{BE1A16E1-3524-4907-8D76-B4CDBC857D00}" name="Column7" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{8D51EA78-35E1-427C-B3AE-93F56E146AB2}" name="Column8" totalsRowFunction="count" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{E826FB71-A68D-434B-AC83-02AB980876B1}" name="Table19" displayName="Table19" ref="A2:H15" headerRowCount="0" headerRowDxfId="200" dataDxfId="198" totalsRowDxfId="199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{E826FB71-A68D-434B-AC83-02AB980876B1}" name="Table19" displayName="Table19" ref="A2:H16" headerRowCount="0" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0BEAA234-F92E-4F4A-B632-8645F359BA3D}" name="Column1" totalsRowLabel="Total" dataDxfId="208"/>
-    <tableColumn id="2" xr3:uid="{42BDD28E-185D-4475-9566-D20E83B801A5}" name="Column2" dataDxfId="207"/>
-    <tableColumn id="3" xr3:uid="{25E263F2-BAF5-463B-9892-BF8276D84894}" name="Column3" dataDxfId="206"/>
-    <tableColumn id="4" xr3:uid="{3BC80FD1-CEF0-4ED6-9D87-A76C08F7BB0F}" name="Column4" dataDxfId="205"/>
-    <tableColumn id="5" xr3:uid="{5E9F19F6-E94E-4B4B-BABE-6D5086FD0015}" name="Column5" dataDxfId="204"/>
-    <tableColumn id="6" xr3:uid="{298D9FE3-A243-43BC-86EA-4F1CA1EF87CE}" name="Column6" dataDxfId="203"/>
-    <tableColumn id="7" xr3:uid="{DFC9E0F1-FC21-47E5-9FB9-B9CA878B08FC}" name="Column7" dataDxfId="202"/>
-    <tableColumn id="8" xr3:uid="{B2530FC7-511E-47A7-8679-EBC4178319DC}" name="Column8" totalsRowFunction="count" dataDxfId="201"/>
+    <tableColumn id="1" xr3:uid="{0BEAA234-F92E-4F4A-B632-8645F359BA3D}" name="Column1" totalsRowLabel="Total" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{42BDD28E-185D-4475-9566-D20E83B801A5}" name="Column2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{25E263F2-BAF5-463B-9892-BF8276D84894}" name="Column3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3BC80FD1-CEF0-4ED6-9D87-A76C08F7BB0F}" name="Column4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{5E9F19F6-E94E-4B4B-BABE-6D5086FD0015}" name="Column5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{298D9FE3-A243-43BC-86EA-4F1CA1EF87CE}" name="Column6" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{DFC9E0F1-FC21-47E5-9FB9-B9CA878B08FC}" name="Column7" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{B2530FC7-511E-47A7-8679-EBC4178319DC}" name="Column8" totalsRowFunction="count" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{1C5F2119-C430-4D29-894E-9FB4FE3BC679}" name="Table02" displayName="Table02" ref="A2:H15" headerRowCount="0" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{1C5F2119-C430-4D29-894E-9FB4FE3BC679}" name="Table02" displayName="Table02" ref="A2:H16" headerRowCount="0" headerRowDxfId="208" dataDxfId="207" totalsRowDxfId="206">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A354EB93-F024-4EB5-B1D9-F96CBFC028D1}" name="Column1" totalsRowLabel="Total" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{8752FF85-2366-46B9-B32D-28DBE0B131CF}" name="Column2" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{B367B66C-919E-4530-8467-2981FCE30C30}" name="Column3" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{98983319-F846-49CC-9CE3-F1ABBFB0C6CD}" name="Column4" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{A351094C-2B30-456C-8A2B-5D09DB01143C}" name="Column5" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{201398B6-531D-4B9C-ACAF-8F9F72F15F88}" name="Column6" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{2A47F542-DF4D-4FC0-B177-523F946653E2}" name="Column7" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{4741BED9-2751-4DFB-95A4-9442B9A297C3}" name="Column8" totalsRowFunction="count" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{A354EB93-F024-4EB5-B1D9-F96CBFC028D1}" name="Column1" totalsRowLabel="Total" dataDxfId="205"/>
+    <tableColumn id="2" xr3:uid="{8752FF85-2366-46B9-B32D-28DBE0B131CF}" name="Column2" dataDxfId="204"/>
+    <tableColumn id="3" xr3:uid="{B367B66C-919E-4530-8467-2981FCE30C30}" name="Column3" dataDxfId="203"/>
+    <tableColumn id="4" xr3:uid="{98983319-F846-49CC-9CE3-F1ABBFB0C6CD}" name="Column4" dataDxfId="202"/>
+    <tableColumn id="5" xr3:uid="{A351094C-2B30-456C-8A2B-5D09DB01143C}" name="Column5" dataDxfId="201"/>
+    <tableColumn id="6" xr3:uid="{201398B6-531D-4B9C-ACAF-8F9F72F15F88}" name="Column6" dataDxfId="200"/>
+    <tableColumn id="7" xr3:uid="{2A47F542-DF4D-4FC0-B177-523F946653E2}" name="Column7" dataDxfId="199"/>
+    <tableColumn id="8" xr3:uid="{4741BED9-2751-4DFB-95A4-9442B9A297C3}" name="Column8" totalsRowFunction="count" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{1C5CD2FC-CA78-40A1-89A6-6BBB638D01B6}" name="Table20" displayName="Table20" ref="A2:H15" headerRowCount="0" headerRowDxfId="211" dataDxfId="209" totalsRowDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{1C5CD2FC-CA78-40A1-89A6-6BBB638D01B6}" name="Table20" displayName="Table20" ref="A2:H16" headerRowCount="0" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A03D23AB-E7F9-4DE3-B649-7172ABE0CDBD}" name="Column1" totalsRowLabel="Total" dataDxfId="219"/>
-    <tableColumn id="2" xr3:uid="{A4F1191A-5033-495C-B140-BBEE5A25B274}" name="Column2" dataDxfId="218"/>
-    <tableColumn id="3" xr3:uid="{77DA7D3E-2DE4-49D2-90AD-58F112045652}" name="Column3" dataDxfId="217"/>
-    <tableColumn id="4" xr3:uid="{00E36786-AA10-4481-B963-ED98F0B031F3}" name="Column4" dataDxfId="216"/>
-    <tableColumn id="5" xr3:uid="{F0E572F1-8242-4118-B9A7-09E5205710C1}" name="Column5" dataDxfId="215"/>
-    <tableColumn id="6" xr3:uid="{625642EA-5518-47B1-B92C-D2DF77AFC50C}" name="Column6" dataDxfId="214"/>
-    <tableColumn id="7" xr3:uid="{9B5DFF62-334A-4022-A60C-D730150D80C7}" name="Column7" dataDxfId="213"/>
-    <tableColumn id="8" xr3:uid="{5BB76A4B-D39F-41B7-9342-F628A88F8100}" name="Column8" totalsRowFunction="count" dataDxfId="212"/>
+    <tableColumn id="1" xr3:uid="{A03D23AB-E7F9-4DE3-B649-7172ABE0CDBD}" name="Column1" totalsRowLabel="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A4F1191A-5033-495C-B140-BBEE5A25B274}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{77DA7D3E-2DE4-49D2-90AD-58F112045652}" name="Column3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00E36786-AA10-4481-B963-ED98F0B031F3}" name="Column4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{F0E572F1-8242-4118-B9A7-09E5205710C1}" name="Column5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{625642EA-5518-47B1-B92C-D2DF77AFC50C}" name="Column6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{9B5DFF62-334A-4022-A60C-D730150D80C7}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5BB76A4B-D39F-41B7-9342-F628A88F8100}" name="Column8" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{40978BA6-21AB-402F-B782-93D5318C035F}" name="Table03" displayName="Table03" ref="A2:H15" headerRowCount="0" headerRowDxfId="24" dataDxfId="22" totalsRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{40978BA6-21AB-402F-B782-93D5318C035F}" name="Table03" displayName="Table03" ref="A2:H16" headerRowCount="0" headerRowDxfId="197" dataDxfId="196" totalsRowDxfId="195">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{21B76265-4292-409E-BC08-9A6638754A60}" name="Column1" totalsRowLabel="Total" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{D8175924-313A-4839-8B49-39ACFB183DBA}" name="Column2" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{568BE577-2ED8-452E-B244-59A89ED3393D}" name="Column3" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{F4D2A3BA-58D1-49D2-AD63-96B736428A89}" name="Column4" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{7675D4B0-1BD8-41E8-996E-4B33065168AE}" name="Column5" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{EAECDA8E-345C-4F91-BD5A-94D2750689CE}" name="Column6" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{98C7D3CB-091A-412C-A47F-17B4CE5F0227}" name="Column7" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{81E7D288-ADC6-468A-BD91-E7C75746CACE}" name="Column8" totalsRowFunction="count" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{21B76265-4292-409E-BC08-9A6638754A60}" name="Column1" totalsRowLabel="Total" dataDxfId="194"/>
+    <tableColumn id="2" xr3:uid="{D8175924-313A-4839-8B49-39ACFB183DBA}" name="Column2" dataDxfId="193"/>
+    <tableColumn id="3" xr3:uid="{568BE577-2ED8-452E-B244-59A89ED3393D}" name="Column3" dataDxfId="192"/>
+    <tableColumn id="4" xr3:uid="{F4D2A3BA-58D1-49D2-AD63-96B736428A89}" name="Column4" dataDxfId="191"/>
+    <tableColumn id="5" xr3:uid="{7675D4B0-1BD8-41E8-996E-4B33065168AE}" name="Column5" dataDxfId="190"/>
+    <tableColumn id="6" xr3:uid="{EAECDA8E-345C-4F91-BD5A-94D2750689CE}" name="Column6" dataDxfId="189"/>
+    <tableColumn id="7" xr3:uid="{98C7D3CB-091A-412C-A47F-17B4CE5F0227}" name="Column7" dataDxfId="188"/>
+    <tableColumn id="8" xr3:uid="{81E7D288-ADC6-468A-BD91-E7C75746CACE}" name="Column8" totalsRowFunction="count" dataDxfId="187"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4FF66500-B6CB-46D4-BEE7-DA1FC6C0FA5A}" name="Table04" displayName="Table04" ref="A2:H15" headerRowCount="0" headerRowDxfId="35" dataDxfId="33" totalsRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4FF66500-B6CB-46D4-BEE7-DA1FC6C0FA5A}" name="Table04" displayName="Table04" ref="A2:H16" headerRowCount="0" headerRowDxfId="186" dataDxfId="185" totalsRowDxfId="184">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BC5353EA-5D1C-4FC6-A518-DA05CFEDE67C}" name="Column1" totalsRowLabel="Total" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{7E5CDA0C-6145-408E-83D3-46BDD16A138B}" name="Column2" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{C5FF176C-EF4F-498D-B19E-611658FDC51C}" name="Column3" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{857D1448-7D7A-4413-B2CB-BDED01E5CBF9}" name="Column4" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{94C72F7F-D767-4E4D-8A0F-BB05C50CE950}" name="Column5" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{35A97619-1358-4100-B549-A9B17F1FE9F2}" name="Column6" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{B9E02800-C281-4FAE-BC79-443B1B598D05}" name="Column7" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{F39BE9BC-CD87-4C30-B3ED-5BE18FCFE040}" name="Column8" totalsRowFunction="count" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{BC5353EA-5D1C-4FC6-A518-DA05CFEDE67C}" name="Column1" totalsRowLabel="Total" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{7E5CDA0C-6145-408E-83D3-46BDD16A138B}" name="Column2" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{C5FF176C-EF4F-498D-B19E-611658FDC51C}" name="Column3" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{857D1448-7D7A-4413-B2CB-BDED01E5CBF9}" name="Column4" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{94C72F7F-D767-4E4D-8A0F-BB05C50CE950}" name="Column5" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{35A97619-1358-4100-B549-A9B17F1FE9F2}" name="Column6" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{B9E02800-C281-4FAE-BC79-443B1B598D05}" name="Column7" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{F39BE9BC-CD87-4C30-B3ED-5BE18FCFE040}" name="Column8" totalsRowFunction="count" dataDxfId="176"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38036769-5661-4F88-8226-829C5FBEBDB3}" name="Table05" displayName="Table05" ref="A2:H15" headerRowCount="0" headerRowDxfId="46" dataDxfId="44" totalsRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38036769-5661-4F88-8226-829C5FBEBDB3}" name="Table05" displayName="Table05" ref="A2:H16" headerRowCount="0" headerRowDxfId="175" dataDxfId="174" totalsRowDxfId="173">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{DFC8CC9F-F86A-44A2-A251-796CFAC8FD74}" name="Column1" totalsRowLabel="Total" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{3992A14F-15A5-4855-9E63-85BBA488EFCF}" name="Column2" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{18F7DA1C-5519-4CAA-8C2F-5DE12FF5824F}" name="Column3" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{2E42620A-1120-4B5A-990D-BA59669F818E}" name="Column4" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{46B2E6DF-6A43-4439-A190-F6C844AAE6CE}" name="Column5" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{602D95B2-A84E-4F23-A475-EA45A9A11AE8}" name="Column6" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{65998936-923D-48A0-89AC-15D0E52AB719}" name="Column7" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{E3D3940D-11F4-458C-88C7-9F3D49FBDCD1}" name="Column8" totalsRowFunction="count" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{DFC8CC9F-F86A-44A2-A251-796CFAC8FD74}" name="Column1" totalsRowLabel="Total" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{3992A14F-15A5-4855-9E63-85BBA488EFCF}" name="Column2" dataDxfId="171"/>
+    <tableColumn id="3" xr3:uid="{18F7DA1C-5519-4CAA-8C2F-5DE12FF5824F}" name="Column3" dataDxfId="170"/>
+    <tableColumn id="4" xr3:uid="{2E42620A-1120-4B5A-990D-BA59669F818E}" name="Column4" dataDxfId="169"/>
+    <tableColumn id="5" xr3:uid="{46B2E6DF-6A43-4439-A190-F6C844AAE6CE}" name="Column5" dataDxfId="168"/>
+    <tableColumn id="6" xr3:uid="{602D95B2-A84E-4F23-A475-EA45A9A11AE8}" name="Column6" dataDxfId="167"/>
+    <tableColumn id="7" xr3:uid="{65998936-923D-48A0-89AC-15D0E52AB719}" name="Column7" dataDxfId="166"/>
+    <tableColumn id="8" xr3:uid="{E3D3940D-11F4-458C-88C7-9F3D49FBDCD1}" name="Column8" totalsRowFunction="count" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{40316C2D-8F9D-4965-83F4-088889FA6E4E}" name="Table06" displayName="Table06" ref="A2:H15" headerRowCount="0" headerRowDxfId="57" dataDxfId="55" totalsRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{40316C2D-8F9D-4965-83F4-088889FA6E4E}" name="Table06" displayName="Table06" ref="A2:H16" headerRowCount="0" headerRowDxfId="164" dataDxfId="163" totalsRowDxfId="162">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{14AE95A6-9473-483F-9AD7-3B2DD396030C}" name="Column1" totalsRowLabel="Total" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{32BFE903-9A19-4325-B7DC-31DD0909E352}" name="Column2" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{8BA83891-5FB3-4CC3-B19E-9C2300BC37A9}" name="Column3" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{3BA65012-6A04-419D-9AB9-8AC0A02D4D0A}" name="Column4" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{E3B02E93-6465-425F-8624-2ED3207327B3}" name="Column5" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{E04B1A11-A7A4-4425-A276-022DD1CF34DB}" name="Column6" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{3C983B8A-E9CC-462A-8F4B-FABADCEF2476}" name="Column7" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{8A22B2CE-8399-43CB-8875-0CDCF802DD24}" name="Column8" totalsRowFunction="count" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{14AE95A6-9473-483F-9AD7-3B2DD396030C}" name="Column1" totalsRowLabel="Total" dataDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{32BFE903-9A19-4325-B7DC-31DD0909E352}" name="Column2" dataDxfId="160"/>
+    <tableColumn id="3" xr3:uid="{8BA83891-5FB3-4CC3-B19E-9C2300BC37A9}" name="Column3" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{3BA65012-6A04-419D-9AB9-8AC0A02D4D0A}" name="Column4" dataDxfId="158"/>
+    <tableColumn id="5" xr3:uid="{E3B02E93-6465-425F-8624-2ED3207327B3}" name="Column5" dataDxfId="157"/>
+    <tableColumn id="6" xr3:uid="{E04B1A11-A7A4-4425-A276-022DD1CF34DB}" name="Column6" dataDxfId="156"/>
+    <tableColumn id="7" xr3:uid="{3C983B8A-E9CC-462A-8F4B-FABADCEF2476}" name="Column7" dataDxfId="155"/>
+    <tableColumn id="8" xr3:uid="{8A22B2CE-8399-43CB-8875-0CDCF802DD24}" name="Column8" totalsRowFunction="count" dataDxfId="154"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5B9F7BEB-6855-49E5-8921-8C49459B56C4}" name="Table07" displayName="Table07" ref="A2:H15" headerRowCount="0" headerRowDxfId="68" dataDxfId="66" totalsRowDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5B9F7BEB-6855-49E5-8921-8C49459B56C4}" name="Table07" displayName="Table07" ref="A2:H16" headerRowCount="0" headerRowDxfId="153" dataDxfId="152" totalsRowDxfId="151">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FDDB1D4-7081-4536-8B24-413452242E18}" name="Column1" totalsRowLabel="Total" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{6C5F00E3-62A3-4D77-8830-CE9E79708F5E}" name="Column2" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{A3A793C2-AB2C-404E-8838-8DCCF3BD807F}" name="Column3" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{3A21DF25-AA93-4D69-BEED-ACD887D07DFD}" name="Column4" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{A80EFE5B-7A1B-4547-9C21-659C5B4CA530}" name="Column5" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{098949CD-E043-4277-ACC0-D3E67FF6CE5B}" name="Column6" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{E6C607E5-C2D3-4114-8948-CA15B39B26F0}" name="Column7" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{6BF48FA3-B2CC-4FB8-9E6F-5F59DB05848F}" name="Column8" totalsRowFunction="count" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{4FDDB1D4-7081-4536-8B24-413452242E18}" name="Column1" totalsRowLabel="Total" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{6C5F00E3-62A3-4D77-8830-CE9E79708F5E}" name="Column2" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{A3A793C2-AB2C-404E-8838-8DCCF3BD807F}" name="Column3" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{3A21DF25-AA93-4D69-BEED-ACD887D07DFD}" name="Column4" dataDxfId="147"/>
+    <tableColumn id="5" xr3:uid="{A80EFE5B-7A1B-4547-9C21-659C5B4CA530}" name="Column5" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{098949CD-E043-4277-ACC0-D3E67FF6CE5B}" name="Column6" dataDxfId="145"/>
+    <tableColumn id="7" xr3:uid="{E6C607E5-C2D3-4114-8948-CA15B39B26F0}" name="Column7" dataDxfId="144"/>
+    <tableColumn id="8" xr3:uid="{6BF48FA3-B2CC-4FB8-9E6F-5F59DB05848F}" name="Column8" totalsRowFunction="count" dataDxfId="143"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4570B26F-C9F6-4F39-9D46-B438AAA491E2}" name="Table08" displayName="Table08" ref="A2:H15" headerRowCount="0" headerRowDxfId="79" dataDxfId="77" totalsRowDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4570B26F-C9F6-4F39-9D46-B438AAA491E2}" name="Table08" displayName="Table08" ref="A2:H16" headerRowCount="0" headerRowDxfId="142" dataDxfId="141" totalsRowDxfId="140">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AC8E3F09-CA02-4473-8C80-00B3B4AF2002}" name="Column1" totalsRowLabel="Total" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{3A2F0AE2-21D4-4742-8459-1E0B3B3EAEB7}" name="Column2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{18F0C809-DA88-47EF-AA91-176E92EAC8D0}" name="Column3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{CC8077B7-B30D-41E0-96FB-A1C5BEB85F6C}" name="Column4" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{12DB422E-90F0-4667-B749-8B26A7DF8CD9}" name="Column5" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{B7217B46-6CFA-4766-9507-1E21DAE234AF}" name="Column6" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{DF6C9D3A-0016-4C91-95D3-FEE5A7A41004}" name="Column7" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{5FD2C978-A389-4D30-A244-74A3EB4CA112}" name="Column8" totalsRowFunction="count" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{AC8E3F09-CA02-4473-8C80-00B3B4AF2002}" name="Column1" totalsRowLabel="Total" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{3A2F0AE2-21D4-4742-8459-1E0B3B3EAEB7}" name="Column2" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{18F0C809-DA88-47EF-AA91-176E92EAC8D0}" name="Column3" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{CC8077B7-B30D-41E0-96FB-A1C5BEB85F6C}" name="Column4" dataDxfId="136"/>
+    <tableColumn id="5" xr3:uid="{12DB422E-90F0-4667-B749-8B26A7DF8CD9}" name="Column5" dataDxfId="135"/>
+    <tableColumn id="6" xr3:uid="{B7217B46-6CFA-4766-9507-1E21DAE234AF}" name="Column6" dataDxfId="134"/>
+    <tableColumn id="7" xr3:uid="{DF6C9D3A-0016-4C91-95D3-FEE5A7A41004}" name="Column7" dataDxfId="133"/>
+    <tableColumn id="8" xr3:uid="{5FD2C978-A389-4D30-A244-74A3EB4CA112}" name="Column8" totalsRowFunction="count" dataDxfId="132"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C036257-763A-485A-A438-08FAAB9042CD}" name="Table09" displayName="Table09" ref="A2:H15" headerRowCount="0" headerRowDxfId="90" dataDxfId="88" totalsRowDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C036257-763A-485A-A438-08FAAB9042CD}" name="Table09" displayName="Table09" ref="A2:H16" headerRowCount="0" headerRowDxfId="131" dataDxfId="130" totalsRowDxfId="129">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2953577D-8AC9-4C5D-98E5-297FE853746D}" name="Column1" totalsRowLabel="Total" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{E41118D4-7019-4BF3-9FFF-31135BB2649B}" name="Column2" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{66ABB05E-75F4-43D3-AF06-16576553C0D8}" name="Column3" dataDxfId="96"/>
-    <tableColumn id="4" xr3:uid="{AAEF8528-74F6-477C-B877-6BC5AE363C6C}" name="Column4" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{08761433-5550-499F-B46A-ABA19B255944}" name="Column5" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{7F800FFD-3713-46EB-8191-2298F803BCA3}" name="Column6" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{FA54EC0B-A4CE-439B-8BBB-B15A3321AF4E}" name="Column7" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{1068926C-D9C5-4111-8C86-8C0E6D3EC527}" name="Column8" totalsRowFunction="count" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{2953577D-8AC9-4C5D-98E5-297FE853746D}" name="Column1" totalsRowLabel="Total" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{E41118D4-7019-4BF3-9FFF-31135BB2649B}" name="Column2" dataDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{66ABB05E-75F4-43D3-AF06-16576553C0D8}" name="Column3" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{AAEF8528-74F6-477C-B877-6BC5AE363C6C}" name="Column4" dataDxfId="125"/>
+    <tableColumn id="5" xr3:uid="{08761433-5550-499F-B46A-ABA19B255944}" name="Column5" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{7F800FFD-3713-46EB-8191-2298F803BCA3}" name="Column6" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{FA54EC0B-A4CE-439B-8BBB-B15A3321AF4E}" name="Column7" dataDxfId="122"/>
+    <tableColumn id="8" xr3:uid="{1068926C-D9C5-4111-8C86-8C0E6D3EC527}" name="Column8" totalsRowFunction="count" dataDxfId="121"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1371,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,14 +1513,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1532,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7506C2E9-4ADB-416C-98DB-75E248FA3024}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,14 +1681,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1690,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7774BF-49E4-4BF2-8FB3-15514453C0F9}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,14 +1849,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1848,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AE63C8-12C4-4201-A910-13A8DE437B43}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,14 +2017,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2006,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29360DA7-3ECC-4F4C-969B-083D464D76C9}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,14 +2185,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2164,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E130CB-78EB-43DE-9D00-E2DFD9323723}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="A2:H15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,14 +2353,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2322,10 +2382,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4F6E61-A627-49EC-9347-405B2B536223}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,14 +2521,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,10 +2550,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B942B55-3700-4DA9-AF2A-D273A97BEDC2}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,14 +2689,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2638,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE93D35-3DAF-42C7-80C7-1D9147AE1385}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,14 +2857,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2796,10 +2886,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A55B06-4E73-4C33-A4BD-C49CD797A133}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,14 +3025,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2954,10 +3054,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9F744E-9E85-495A-B097-29ED0E209199}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,14 +3193,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3112,10 +3222,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA67A9E1-47E6-40BF-A0DF-8F4ED24C7AC4}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,14 +3364,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3274,10 +3394,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E01DD4-7668-4AC1-B0EC-A4B09E804AD0}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3416,14 +3536,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3436,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C08C48F-FCBF-4B2B-921E-F0D0BF71C39A}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="A2:H15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,14 +3708,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3597,10 +3737,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DCB708-AF82-4DCB-901E-589C73705F6B}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,14 +3879,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3758,10 +3908,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7A0DDD-3D00-4E83-9FFC-4804FB1B335A}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,14 +4050,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3919,10 +4079,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC935D5-0BFD-49AC-A36E-2A985F47D5F1}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,14 +4218,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4077,10 +4247,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6702ADDA-50E0-4C31-9C32-D51896D11674}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4216,14 +4386,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4235,10 +4415,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1153DC95-A0C4-4A68-89A1-A398F4F60620}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,14 +4554,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4393,10 +4583,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88D364C-D414-4EAD-B036-56ABA4638968}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4532,14 +4722,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>